<commit_message>
Update test cases and fix checkout flow
</commit_message>
<xml_diff>
--- a/API Testing.xlsx
+++ b/API Testing.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abanoub Melad\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f096b8a72b43649a/سطح المكتب/New folder/Test_Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_6D1F3CCA3DC80D5675D62DA4D052E3D4591F772F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BC0F770-B26C-40BD-AB8F-AA4D218192B6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test_Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Test_Cases" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,55 +26,62 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="6">
+  <futureMetadata name="XLRICHVALUE" count="7">
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="0"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="1"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="2"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="3"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="4"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="5"/>
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="6"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="6">
+  <valueMetadata count="7">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -90,13 +99,16 @@
     </bk>
     <bk>
       <rc t="1" v="5"/>
+    </bk>
+    <bk>
+      <rc t="1" v="6"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>TC_ID</t>
   </si>
@@ -230,24 +242,63 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Final Result</t>
+  </si>
+  <si>
+    <t>Project Name:</t>
+  </si>
+  <si>
+    <t>E-Commerce</t>
+  </si>
+  <si>
+    <t>Client:</t>
+  </si>
+  <si>
+    <t>Created By:</t>
+  </si>
+  <si>
+    <t>Team 53 "CTRL+ALT+DEFECT"</t>
+  </si>
+  <si>
+    <t>Creation Date:</t>
+  </si>
+  <si>
+    <t>Reviewed by:</t>
+  </si>
+  <si>
+    <t>Ahmed Essam</t>
+  </si>
+  <si>
+    <t>Type of Testing:</t>
+  </si>
+  <si>
+    <t>API Testing</t>
+  </si>
+  <si>
+    <t>29/11/2025</t>
+  </si>
+  <si>
+    <t>https://gorest.co.in/#google_vignette</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -255,7 +306,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -263,7 +314,7 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -271,9 +322,23 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -296,7 +361,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -319,13 +384,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -353,11 +455,32 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -419,7 +542,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="6">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="7">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -444,6 +567,10 @@
     <v>5</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>6</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -464,6 +591,7 @@
   <rel r:id="rId4"/>
   <rel r:id="rId5"/>
   <rel r:id="rId6"/>
+  <rel r:id="rId7"/>
 </richValueRels>
 </file>
 
@@ -729,32 +857,103 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E6A80D-2026-4CD3-B2FA-CBEB9B608E89}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="35.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="32" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.44140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="31" style="1" customWidth="1"/>
-    <col min="10" max="10" width="26.21875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="33" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5546875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="1" width="21.09765625" customWidth="1"/>
+    <col min="2" max="2" width="32.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="46.8" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="78" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="31.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" location="google_vignette" xr:uid="{5B42177E-DD3D-4286-BDC6-90B416F6657D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.19921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.69921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35.09765625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.59765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.19921875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.3984375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="31" style="1" customWidth="1"/>
+    <col min="10" max="10" width="26.19921875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="33" style="2" customWidth="1"/>
+    <col min="12" max="12" width="15.296875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="19.59765625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="48.796875" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -794,8 +993,11 @@
       <c r="M1" s="10" t="s">
         <v>38</v>
       </c>
+      <c r="N1" s="10" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="94.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -835,8 +1037,11 @@
       <c r="M2" s="2" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
+      <c r="N2" s="11" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -873,11 +1078,12 @@
       <c r="L3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="2" t="e" vm="3">
+      <c r="M3" s="2" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
+      <c r="N3" s="12"/>
     </row>
-    <row r="4" spans="1:13" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="61.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -896,7 +1102,7 @@
       <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="2" t="e" vm="4">
+      <c r="G4" s="2" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
       <c r="H4" s="2">
@@ -914,11 +1120,12 @@
       <c r="L4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="2" t="e" vm="5">
+      <c r="M4" s="2" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
+      <c r="N4" s="12"/>
     </row>
-    <row r="5" spans="1:13" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="73.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -955,19 +1162,23 @@
       <c r="L5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="2" t="e" vm="6">
+      <c r="M5" s="2" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
+      <c r="N5" s="13"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="N2:N5"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>